<commit_message>
Fix comparison: Add freee申告 detailed information
- Added freee申告 (tax filing) as major advantage for freee
- New sheet: freee申告 詳細 with all plans and pricing
- Updated tax filing comparison: MF has no built-in tax software
- freee申告 法人税: 29,800円〜/year
- freee申告 消費税: included with freee会計
- freee申告 償却資産: 59,800円/year

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/ms-expense-app/docs/mf-freee-comparison.xlsx
+++ b/ms-expense-app/docs/mf-freee-comparison.xlsx
@@ -10,13 +10,14 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="総合比較" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="会計入力・記帳" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="税務申告" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="償却資産申告" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="給与・年末調整・労務" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="経費精算" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="請求・支払" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="料金プラン" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="市場シェア" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="推奨シナリオ" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="freee申告 詳細" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="償却資産申告" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="給与・年末調整・労務" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="経費精算" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="請求・支払" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="料金プラン" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="市場シェア" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="推奨シナリオ" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -26,7 +27,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -64,8 +65,12 @@
       <color rgb="0000AA4F"/>
       <sz val="12"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -76,6 +81,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00F8F9FA"/>
         <bgColor rgb="00F8F9FA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E6F7ED"/>
+        <bgColor rgb="00E6F7ED"/>
       </patternFill>
     </fill>
   </fills>
@@ -97,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -116,16 +127,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -581,22 +594,22 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>税務申告連携</t>
+          <t>税務申告（自社完結）</t>
         </is>
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
+          <t>★★☆☆☆</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
           <t>★★★★★</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>★★★★☆</t>
-        </is>
-      </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>MFは達人とAPI連携強化</t>
+          <t>freeeは freee申告で自社完結</t>
         </is>
       </c>
     </row>
@@ -724,7 +737,232 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>クラウド会計ソフト市場シェア（2025年）</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="inlineStr">
+        <is>
+          <t>【法人向けクラウド会計シェア】</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>ソフト</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>シェア</t>
+        </is>
+      </c>
+      <c r="C4" s="7" t="inlineStr">
+        <is>
+          <t>順位</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="12" t="inlineStr">
+        <is>
+          <t>freee</t>
+        </is>
+      </c>
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>32.3%</t>
+        </is>
+      </c>
+      <c r="C5" s="12" t="inlineStr">
+        <is>
+          <t>1位</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="12" t="inlineStr">
+        <is>
+          <t>マネーフォワード</t>
+        </is>
+      </c>
+      <c r="B6" s="12" t="inlineStr">
+        <is>
+          <t>19.2%</t>
+        </is>
+      </c>
+      <c r="C6" s="12" t="inlineStr">
+        <is>
+          <t>2位</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="12" t="inlineStr">
+        <is>
+          <t>弥生シリーズ</t>
+        </is>
+      </c>
+      <c r="B7" s="12" t="inlineStr">
+        <is>
+          <t>15.4%</t>
+        </is>
+      </c>
+      <c r="C7" s="12" t="inlineStr">
+        <is>
+          <t>3位</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="12" t="inlineStr">
+        <is>
+          <t>その他</t>
+        </is>
+      </c>
+      <c r="B8" s="12" t="inlineStr">
+        <is>
+          <t>33.1%</t>
+        </is>
+      </c>
+      <c r="C8" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="9" t="inlineStr">
+        <is>
+          <t>【個人事業主向けシェア】</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>ソフト</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>シェア</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>順位</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="12" t="inlineStr">
+        <is>
+          <t>弥生シリーズ</t>
+        </is>
+      </c>
+      <c r="B13" s="12" t="inlineStr">
+        <is>
+          <t>55.4%</t>
+        </is>
+      </c>
+      <c r="C13" s="12" t="inlineStr">
+        <is>
+          <t>1位</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="12" t="inlineStr">
+        <is>
+          <t>freee</t>
+        </is>
+      </c>
+      <c r="B14" s="12" t="inlineStr">
+        <is>
+          <t>24.0%</t>
+        </is>
+      </c>
+      <c r="C14" s="12" t="inlineStr">
+        <is>
+          <t>2位</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="12" t="inlineStr">
+        <is>
+          <t>マネーフォワード</t>
+        </is>
+      </c>
+      <c r="B15" s="12" t="inlineStr">
+        <is>
+          <t>14.3%</t>
+        </is>
+      </c>
+      <c r="C15" s="12" t="inlineStr">
+        <is>
+          <t>3位</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="12" t="inlineStr">
+        <is>
+          <t>その他</t>
+        </is>
+      </c>
+      <c r="B16" s="12" t="inlineStr">
+        <is>
+          <t>6.3%</t>
+        </is>
+      </c>
+      <c r="C16" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>出典: MM総研 2025年3月末調査</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -744,12 +982,12 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="12" t="inlineStr">
+      <c r="A3" s="13" t="inlineStr">
         <is>
           <t>マネーフォワードが向いているケース</t>
         </is>
       </c>
-      <c r="B3" s="13" t="inlineStr">
+      <c r="B3" s="14" t="inlineStr">
         <is>
           <t>freeeが向いているケース</t>
         </is>
@@ -835,7 +1073,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>・償却資産申告まで一貫対応したい</t>
+          <t>・会計から税務申告まで自社完結したい</t>
         </is>
       </c>
     </row>
@@ -847,13 +1085,56 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>・達人シリーズを持っていない（新規導入）</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>・税務申告は達人シリーズで行う前提</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>・API連携で独自システムと接続</t>
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" s="15" t="inlineStr">
+        <is>
+          <t>【会計事務所としての結論】</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>freeeは「freee申告」で税務申告まで自社完結できるのが大きな強み。</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>達人シリーズを既に導入済みの事務所はMFでも問題ないが、新規導入ならfreeeが有利。</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>顧問先の規模・業種・ITリテラシーに応じて使い分けるのが現実的。</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1062,7 +1343,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1070,9 +1351,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="35" customWidth="1" min="2" max="2"/>
-    <col width="35" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="1" max="1"/>
+    <col width="38" customWidth="1" min="2" max="2"/>
+    <col width="38" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -1113,19 +1394,20 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>外部連携（達人シリーズ等）
-API連携で自動データ取込</t>
+          <t>× 自社機能なし
+外部連携（達人シリーズ等）が必要</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>外部連携（達人シリーズ等）
-CSV/API連携対応</t>
+          <t>◎ freee申告（法人税）
+自社ソフトで完結可能
+年額29,800円〜</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>MF優位</t>
+          <t>freee優位</t>
         </is>
       </c>
     </row>
@@ -1137,37 +1419,39 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>外部連携（消費税の達人等）
-消費税集計データ出力</t>
+          <t>× 自社機能なし
+外部連携（達人シリーズ等）が必要</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>外部連携（消費税の達人等）
-消費税集計データ出力</t>
+          <t>◎ freee申告（消費税）
+freee会計に付帯
+インボイス対応・電子申告可</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>同等</t>
+          <t>freee優位</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>所得税確定申告</t>
+          <t>所得税確定申告
+（個人事業主）</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>クラウド確定申告で完結
+          <t>○ クラウド確定申告で完結
 e-Tax対応</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>確定申告freeeで完結
+          <t>◎ freee会計 確定申告機能
 スマホのみで申告可能</t>
         </is>
       </c>
@@ -1180,46 +1464,116 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>達人シリーズ連携</t>
+          <t>所得税申告
+（税理士向け代理）</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>2024年API連携実装
-ワンクリックでデータ取込</t>
+          <t>× 自社機能なし
+外部連携が必要</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>2013年〜連携対応
-CSV/データ連携</t>
+          <t>◎ freee申告（所得税）
+アドバイザー向け提供</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>MF優位</t>
+          <t>freee優位</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
+          <t>達人シリーズ連携</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>◎ 2024年API連携実装
+ワンクリックでデータ取込</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>○ CSV/データ連携対応
+※freee申告があるため依存度低い</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>MF優位</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
           <t>電子申告対応</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>外部ソフト経由</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>外部ソフト経由</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>同等</t>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>△ 外部ソフト経由のみ</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>◎ freee申告内で完結
+法人税+消費税一括送信可</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>freee優位</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>申告書作成の一体性</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>△ 会計→外部ソフトで申告</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>◎ 会計→申告まで自社完結
+データ自動連携</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>freee優位</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>【重要】freeeは「freee申告」で法人税・消費税・所得税の申告書作成から電子申告まで自社完結可能。</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>マネーフォワードは自社で税務申告ソフトを持たないため、達人シリーズ等の外部ソフトが必須。</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>会計事務所が達人シリーズを既に導入済みの場合はMFでも問題ないが、新規導入ならfreeeが有利。</t>
         </is>
       </c>
     </row>
@@ -1232,6 +1586,264 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>freee申告 プラン・機能一覧</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>プラン名</t>
+        </is>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>年額（税別）</t>
+        </is>
+      </c>
+      <c r="C3" s="8" t="inlineStr">
+        <is>
+          <t>主な機能</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>freee申告 法人税スターター</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>29,800円</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>法人税確定申告
+電子申告対応</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>freee申告 法人税スタンダード</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>48,800円</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>法人税確定申告
++高度な機能</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>freee申告 法人税アドバンス</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>要問合せ</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>資本金1億円超対応
+固定資産100件以上対応</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>freee申告 消費税</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>freee会計に付帯</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>消費税申告書作成
+電子申告・インボイス対応</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>freee申告 所得税</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>アドバイザー向け</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>税理士の代理申告用
+一括電子申告可</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>freee申告 償却資産</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>59,800円</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>償却資産申告書作成
+eLTAX電子申告対応</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>freee申告 内訳書・概況書</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>別途契約</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>勘定科目内訳明細書
+法人事業概況説明書</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>freee申告 年調・法定調書</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>freee人事労務に付帯</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>年末調整
+法定調書合計表</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>【freee申告の強み】</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>・freee会計からデータ自動連携（当期純利益・交際費・固定資産等）</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>・帳票間の数字連携がツリー形式で表示され、整合性確認が容易</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>・法人税+消費税の一括電子申告が可能（アドバイザー向け）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>・eLTAX/e-Taxインストール不要で電子申告可能</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>【注意事項】</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>・資本金1億円超の法人はアドバンスプランが必要</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>・電気・ガス供給業、保険業は対応外（保険代理店は可）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>・修正申告・予定申告はスターター/スタンダードでは不可</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1332,7 +1944,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>△ 外部ソフト連携
+          <t>× 自社機能なし
 減価償却の達人等へデータ出力</t>
         </is>
       </c>
@@ -1356,7 +1968,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>△ 外部ソフト経由</t>
+          <t>× 外部ソフト経由のみ</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -1379,7 +1991,7 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>達人シリーズ等の費用</t>
+          <t>達人シリーズ等の費用が別途必要</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -1389,203 +2001,6 @@
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>条件による</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="35" customWidth="1" min="2" max="2"/>
-    <col width="35" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="6" t="inlineStr">
-        <is>
-          <t>給与・年末調整・労務・社保・法定調書の比較</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="7" t="inlineStr">
-        <is>
-          <t>項目</t>
-        </is>
-      </c>
-      <c r="B3" s="7" t="inlineStr">
-        <is>
-          <t>マネーフォワード</t>
-        </is>
-      </c>
-      <c r="C3" s="7" t="inlineStr">
-        <is>
-          <t>freee</t>
-        </is>
-      </c>
-      <c r="D3" s="7" t="inlineStr">
-        <is>
-          <t>評価</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>給与計算</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>クラウド給与
-勤怠連携対応</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>人事労務freee
-会計と一体型</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>freee優位</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>年末調整</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>クラウド年末調整
-Web完結・e-Tax対応</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>人事労務freee内
-Web完結・e-Tax対応</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>同等</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>社会保険手続き</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>クラウド社会保険
-算定基礎届・月変届出力</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>人事労務freee内
-算定基礎届・月変届出力</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>同等</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>法定調書</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>○ 給与支払報告書・源泉徴収票
-e-Tax/eLTAX連携</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>○ 給与支払報告書・源泉徴収票
-e-Tax/eLTAX連携</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>同等</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
-          <t>外部連携</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>◎ SmartHR、Touch On Time等</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>○ 主要サービス対応</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>MF優位</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>料金</t>
-        </is>
-      </c>
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>基本料金内 or 追加契約</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="inlineStr">
-        <is>
-          <t>月額2,600円〜（5名まで）</t>
-        </is>
-      </c>
-      <c r="D9" s="3" t="inlineStr">
         <is>
           <t>条件による</t>
         </is>
@@ -1622,7 +2037,7 @@
     <row r="1">
       <c r="A1" s="6" t="inlineStr">
         <is>
-          <t>経費精算の比較</t>
+          <t>給与・年末調整・労務・社保・法定調書の比較</t>
         </is>
       </c>
     </row>
@@ -1651,17 +2066,19 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>サービス形態</t>
+          <t>給与計算</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>クラウド経費（別契約）</t>
+          <t>クラウド給与
+勤怠連携対応</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>freee会計内蔵 / freee経費精算</t>
+          <t>人事労務freee
+会計と一体型</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -1673,19 +2090,19 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>領収書読取</t>
+          <t>年末調整</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>◎ AI-OCR高精度
-使うほど学習</t>
+          <t>クラウド年末調整
+Web完結・e-Tax対応</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>◎ AI-OCR対応
-税区分・金額自動入力</t>
+          <t>freee申告 年調・法定調書
+人事労務に付帯</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -1697,39 +2114,43 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>申請・承認</t>
+          <t>社会保険手続き</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>○ スマホ完結</t>
+          <t>クラウド社会保険
+算定基礎届・月変届出力</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>◎ スマホ・LINE対応</t>
+          <t>人事労務freee内
+算定基礎届・月変届出力</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>freee優位</t>
+          <t>同等</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>会計連携</t>
+          <t>法定調書</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>○ 仕訳自動計上</t>
+          <t>○ 給与支払報告書・源泉徴収票
+e-Tax/eLTAX連携</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>◎ シームレス連携</t>
+          <t>◎ freee申告 年調・法定調書
+法定調書合計表まで対応</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
@@ -1741,44 +2162,44 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>振込データ作成</t>
+          <t>外部連携</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>○ 対応</t>
+          <t>◎ SmartHR、Touch On Time等</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>○ 対応</t>
+          <t>○ 主要サービス対応</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>同等</t>
+          <t>MF優位</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>電子帳簿保存法</t>
+          <t>料金</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>○ JIIMA認証取得</t>
+          <t>基本料金内 or 追加契約</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>○ JIIMA認証取得</t>
+          <t>月額2,600円〜（5名まで）</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>同等</t>
+          <t>条件による</t>
         </is>
       </c>
     </row>
@@ -1791,6 +2212,197 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="35" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>経費精算の比較</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>項目</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="inlineStr">
+        <is>
+          <t>マネーフォワード</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>freee</t>
+        </is>
+      </c>
+      <c r="D3" s="7" t="inlineStr">
+        <is>
+          <t>評価</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>サービス形態</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>クラウド経費（別契約）</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>freee会計内蔵 / freee経費精算</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>freee優位</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>領収書読取</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>◎ AI-OCR高精度
+使うほど学習</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>◎ AI-OCR対応
+税区分・金額自動入力</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>同等</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>申請・承認</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>○ スマホ完結</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>◎ スマホ・LINE対応</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>freee優位</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>会計連携</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>○ 仕訳自動計上</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>◎ シームレス連携</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>freee優位</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>振込データ作成</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>○ 対応</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>○ 対応</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>同等</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>電子帳簿保存法</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>○ JIIMA認証取得</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>○ JIIMA認証取得</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>同等</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2002,13 +2614,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2017,8 +2629,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
   </cols>
@@ -2031,124 +2643,216 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="inlineStr">
+      <c r="A3" s="9" t="inlineStr">
+        <is>
+          <t>【会計ソフト】</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="inlineStr">
         <is>
           <t>プラン</t>
         </is>
       </c>
-      <c r="B3" s="8" t="inlineStr">
+      <c r="B4" s="10" t="inlineStr">
         <is>
           <t>MF月額</t>
         </is>
       </c>
-      <c r="C3" s="8" t="inlineStr">
+      <c r="C4" s="10" t="inlineStr">
         <is>
           <t>MF年額</t>
         </is>
       </c>
-      <c r="D3" s="8" t="inlineStr">
+      <c r="D4" s="10" t="inlineStr">
         <is>
           <t>freee月額</t>
         </is>
       </c>
-      <c r="E3" s="8" t="inlineStr">
+      <c r="E4" s="10" t="inlineStr">
         <is>
           <t>freee年額</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="9" t="inlineStr">
+    <row r="5">
+      <c r="A5" s="11" t="inlineStr">
         <is>
           <t>スモール/スターター</t>
         </is>
       </c>
-      <c r="B4" s="9" t="inlineStr">
+      <c r="B5" s="11" t="inlineStr">
         <is>
           <t>3,980円</t>
         </is>
       </c>
-      <c r="C4" s="9" t="inlineStr">
+      <c r="C5" s="11" t="inlineStr">
         <is>
           <t>35,760円</t>
         </is>
       </c>
-      <c r="D4" s="9" t="inlineStr">
+      <c r="D5" s="11" t="inlineStr">
         <is>
           <t>4,780円</t>
         </is>
       </c>
-      <c r="E4" s="9" t="inlineStr">
+      <c r="E5" s="11" t="inlineStr">
         <is>
           <t>47,760円</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="9" t="inlineStr">
+    <row r="6">
+      <c r="A6" s="11" t="inlineStr">
         <is>
           <t>ビジネス/スタンダード</t>
         </is>
       </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B6" s="11" t="inlineStr">
         <is>
           <t>5,980円</t>
         </is>
       </c>
-      <c r="C5" s="9" t="inlineStr">
+      <c r="C6" s="11" t="inlineStr">
         <is>
           <t>59,760円</t>
         </is>
       </c>
-      <c r="D5" s="9" t="inlineStr">
+      <c r="D6" s="11" t="inlineStr">
         <is>
           <t>9,280円</t>
         </is>
       </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="E6" s="11" t="inlineStr">
         <is>
           <t>95,760円</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="9" t="inlineStr">
+    <row r="7">
+      <c r="A7" s="11" t="inlineStr">
         <is>
           <t>エンタープライズ等</t>
         </is>
       </c>
-      <c r="B6" s="9" t="inlineStr">
+      <c r="B7" s="11" t="inlineStr">
         <is>
           <t>要問合せ</t>
         </is>
       </c>
-      <c r="C6" s="9" t="inlineStr">
+      <c r="C7" s="11" t="inlineStr">
         <is>
           <t>要問合せ</t>
         </is>
       </c>
-      <c r="D6" s="9" t="inlineStr">
+      <c r="D7" s="11" t="inlineStr">
         <is>
           <t>要問合せ</t>
         </is>
       </c>
-      <c r="E6" s="9" t="inlineStr">
+      <c r="E7" s="11" t="inlineStr">
         <is>
           <t>要問合せ</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="10">
+      <c r="A10" s="9" t="inlineStr">
+        <is>
+          <t>【税務申告ソフト】</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>項目</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>マネーフォワード</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>freee</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>法人税申告</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>自社機能なし
+（達人シリーズ等が別途必要）</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>freee申告 年額29,800円〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>消費税申告</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>自社機能なし
+（達人シリーズ等が別途必要）</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>freee会計に付帯（追加費用なし）</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>償却資産申告</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>自社機能なし
+（達人シリーズ等が別途必要）</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>freee申告 年額59,800円</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>※料金は2025年1月時点。最新料金は各社公式サイトをご確認ください。</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="18">
+      <c r="A18" t="inlineStr">
         <is>
           <t>※freeeは2024年7月に価格改定あり。クラウドソフトは価格改定リスクがあります。</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>※MFで税務申告を行う場合、達人シリーズ等の費用が別途発生します。</t>
         </is>
       </c>
     </row>
@@ -2158,229 +2862,4 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="6" t="inlineStr">
-        <is>
-          <t>クラウド会計ソフト市場シェア（2025年）</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="10" t="inlineStr">
-        <is>
-          <t>【法人向けクラウド会計シェア】</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="7" t="inlineStr">
-        <is>
-          <t>ソフト</t>
-        </is>
-      </c>
-      <c r="B4" s="7" t="inlineStr">
-        <is>
-          <t>シェア</t>
-        </is>
-      </c>
-      <c r="C4" s="7" t="inlineStr">
-        <is>
-          <t>順位</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="inlineStr">
-        <is>
-          <t>freee</t>
-        </is>
-      </c>
-      <c r="B5" s="11" t="inlineStr">
-        <is>
-          <t>32.3%</t>
-        </is>
-      </c>
-      <c r="C5" s="11" t="inlineStr">
-        <is>
-          <t>1位</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="11" t="inlineStr">
-        <is>
-          <t>マネーフォワード</t>
-        </is>
-      </c>
-      <c r="B6" s="11" t="inlineStr">
-        <is>
-          <t>19.2%</t>
-        </is>
-      </c>
-      <c r="C6" s="11" t="inlineStr">
-        <is>
-          <t>2位</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="11" t="inlineStr">
-        <is>
-          <t>弥生シリーズ</t>
-        </is>
-      </c>
-      <c r="B7" s="11" t="inlineStr">
-        <is>
-          <t>15.4%</t>
-        </is>
-      </c>
-      <c r="C7" s="11" t="inlineStr">
-        <is>
-          <t>3位</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="11" t="inlineStr">
-        <is>
-          <t>その他</t>
-        </is>
-      </c>
-      <c r="B8" s="11" t="inlineStr">
-        <is>
-          <t>33.1%</t>
-        </is>
-      </c>
-      <c r="C8" s="11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="10" t="inlineStr">
-        <is>
-          <t>【個人事業主向けシェア】</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="7" t="inlineStr">
-        <is>
-          <t>ソフト</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>シェア</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="inlineStr">
-        <is>
-          <t>順位</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="11" t="inlineStr">
-        <is>
-          <t>弥生シリーズ</t>
-        </is>
-      </c>
-      <c r="B13" s="11" t="inlineStr">
-        <is>
-          <t>55.4%</t>
-        </is>
-      </c>
-      <c r="C13" s="11" t="inlineStr">
-        <is>
-          <t>1位</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="11" t="inlineStr">
-        <is>
-          <t>freee</t>
-        </is>
-      </c>
-      <c r="B14" s="11" t="inlineStr">
-        <is>
-          <t>24.0%</t>
-        </is>
-      </c>
-      <c r="C14" s="11" t="inlineStr">
-        <is>
-          <t>2位</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="11" t="inlineStr">
-        <is>
-          <t>マネーフォワード</t>
-        </is>
-      </c>
-      <c r="B15" s="11" t="inlineStr">
-        <is>
-          <t>14.3%</t>
-        </is>
-      </c>
-      <c r="C15" s="11" t="inlineStr">
-        <is>
-          <t>3位</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="11" t="inlineStr">
-        <is>
-          <t>その他</t>
-        </is>
-      </c>
-      <c r="B16" s="11" t="inlineStr">
-        <is>
-          <t>6.3%</t>
-        </is>
-      </c>
-      <c r="C16" s="11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>出典: MM総研 2025年3月末調査</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>